<commit_message>
Updated the Reconfig Vivado project
</commit_message>
<xml_diff>
--- a/Implementation_Results/Reconfig_Results/Reconfigured_Data.xlsx
+++ b/Implementation_Results/Reconfig_Results/Reconfigured_Data.xlsx
@@ -2905,7 +2905,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C928-4D69-BBB4-0247E9EBD3CA}"/>
+              <c16:uniqueId val="{00000000-81ED-43AD-ACB6-D8DCB69F1D56}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2976,7 +2976,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-C928-4D69-BBB4-0247E9EBD3CA}"/>
+              <c16:uniqueId val="{00000001-81ED-43AD-ACB6-D8DCB69F1D56}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3064,7 +3064,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-C928-4D69-BBB4-0247E9EBD3CA}"/>
+              <c16:uniqueId val="{00000002-81ED-43AD-ACB6-D8DCB69F1D56}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3530,1881 +3530,6 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D4C9-4157-976B-4A1F7D439869}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Reconfigured Adders'!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>LUT count</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Reconfigured Adders'!$A$6:$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Standard RCA</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>RCA_Cut1LUT</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>RCA_Cut2LUTshifted</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>QuAd_1122_0000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Reconfigured Adders'!$D$6:$D$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-D4C9-4157-976B-4A1F7D439869}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="60"/>
-        <c:overlap val="-100"/>
-        <c:axId val="584066536"/>
-        <c:axId val="584061288"/>
-      </c:barChart>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Reconfigured Adders'!$F$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Power in uW</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Reconfigured Adders'!$A$6:$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Standard RCA</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>RCA_Cut1LUT</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>RCA_Cut2LUTshifted</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>QuAd_1122_0000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Reconfigured Adders'!$F$6:$F$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>95.855999999999995</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>221.75899999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>181.24799999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>237.846</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-D4C9-4157-976B-4A1F7D439869}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="260"/>
-        <c:overlap val="100"/>
-        <c:axId val="584129840"/>
-        <c:axId val="584124592"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="584066536"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="584061288"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="584061288"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Delay in ns, LUT</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="de-DE" baseline="0"/>
-                  <a:t> count</a:t>
-                </a:r>
-                <a:endParaRPr lang="de-DE"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="584066536"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="584124592"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="r"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Power in uW</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="584129840"/>
-        <c:crosses val="max"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:catAx>
-        <c:axId val="584129840"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="1"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="584124592"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Reconfigured Adders'!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Delay in ns</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Reconfigured Adders'!$A$10:$A$13</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>RCA_LUT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>RCA_Cut2LUT</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>QuAd_224_000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>QuAd_3113_0000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Reconfigured Adders'!$C$10:$C$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>8.7889999999999997</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.8559999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.6289999999999996</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.66</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3045-4BEA-BDD6-129A17445B07}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Reconfigured Adders'!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>LUT count</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Reconfigured Adders'!$A$10:$A$13</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>RCA_LUT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>RCA_Cut2LUT</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>QuAd_224_000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>QuAd_3113_0000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Reconfigured Adders'!$D$10:$D$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-3045-4BEA-BDD6-129A17445B07}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="60"/>
-        <c:overlap val="-100"/>
-        <c:axId val="584066536"/>
-        <c:axId val="584061288"/>
-      </c:barChart>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Reconfigured Adders'!$F$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Power in uW</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Reconfigured Adders'!$A$10:$A$13</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>RCA_LUT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>RCA_Cut2LUT</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>QuAd_224_000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>QuAd_3113_0000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Reconfigured Adders'!$F$10:$F$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>346.048</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>237.482</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>303.14999999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>295.91000000000003</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-3045-4BEA-BDD6-129A17445B07}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="260"/>
-        <c:overlap val="100"/>
-        <c:axId val="584129840"/>
-        <c:axId val="584124592"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="584066536"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="584061288"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="584061288"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Delay in ns, LUT</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="de-DE" baseline="0"/>
-                  <a:t> count</a:t>
-                </a:r>
-                <a:endParaRPr lang="de-DE"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="584066536"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="584124592"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="r"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Power in uW</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="584129840"/>
-        <c:crosses val="max"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:catAx>
-        <c:axId val="584129840"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="1"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="584124592"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Reconfigured Adders'!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Delay in ns</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Reconfigured Adders'!$A$2:$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>RCA_LUT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>RCA_Cut1LUT</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>QuAd_1111_0000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>RCA_Cut2LUT</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Reconfigured Adders'!$C$2:$C$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>8.8249999999999993</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.8770000000000007</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.1340000000000003</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.5960000000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-81ED-43AD-ACB6-D8DCB69F1D56}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Reconfigured Adders'!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>LUT count</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Reconfigured Adders'!$A$2:$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>RCA_LUT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>RCA_Cut1LUT</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>QuAd_1111_0000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>RCA_Cut2LUT</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Reconfigured Adders'!$D$2:$D$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-81ED-43AD-ACB6-D8DCB69F1D56}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="60"/>
-        <c:overlap val="-100"/>
-        <c:axId val="584066536"/>
-        <c:axId val="584061288"/>
-      </c:barChart>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Reconfigured Adders'!$F$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Power in uW</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Reconfigured Adders'!$A$2:$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>RCA_LUT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>RCA_Cut1LUT</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>QuAd_1111_0000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>RCA_Cut2LUT</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Reconfigured Adders'!$F$2:$F$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>209.18799999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>153.07</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>194.142</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>103.976</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-81ED-43AD-ACB6-D8DCB69F1D56}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="260"/>
-        <c:overlap val="100"/>
-        <c:axId val="584129840"/>
-        <c:axId val="584124592"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="584066536"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="584061288"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="584061288"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Delay in ns, LUT</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="de-DE" baseline="0"/>
-                  <a:t> count</a:t>
-                </a:r>
-                <a:endParaRPr lang="de-DE"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="584066536"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="584124592"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="r"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Power in uW</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="584129840"/>
-        <c:crosses val="max"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:catAx>
-        <c:axId val="584129840"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="1"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="584124592"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Reconfigured Adders'!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Delay in ns</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Reconfigured Adders'!$A$6:$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Standard RCA</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>RCA_Cut1LUT</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>RCA_Cut2LUTshifted</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>QuAd_1122_0000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Reconfigured Adders'!$C$6:$C$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>8.4930000000000003</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.8689999999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.8190000000000008</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.43</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-73B3-4AE0-8433-95432473EF0E}"/>
             </c:ext>
           </c:extLst>
@@ -5942,7 +4067,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -6807,126 +4932,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
   <cs:axisTitle>
@@ -9341,1515 +7346,6 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -11358,14 +7854,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11388,14 +7884,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>781050</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1171575</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11420,14 +7916,14 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11443,100 +7939,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="14" name="Chart 13"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>695325</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>695325</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="15" name="Chart 14"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>800100</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="16" name="Chart 15"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -11912,7 +8314,7 @@
   <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>